<commit_message>
Create TRF by external user
</commit_message>
<xml_diff>
--- a/trf-internal-user.xlsx
+++ b/trf-internal-user.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19540" windowHeight="5650" tabRatio="438"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19540" windowHeight="5650" tabRatio="643"/>
   </bookViews>
   <sheets>
     <sheet name="temp" sheetId="19" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1341" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="172">
   <si>
     <t>Specimen ID Number</t>
   </si>
@@ -546,13 +546,19 @@
     <t>2000008</t>
   </si>
   <si>
-    <t>2000084</t>
-  </si>
-  <si>
-    <t>2000085</t>
-  </si>
-  <si>
     <t>submit</t>
+  </si>
+  <si>
+    <t>select_search</t>
+  </si>
+  <si>
+    <t>Clinic Name</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>1000092</t>
   </si>
 </sst>
 </file>
@@ -1427,10 +1433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH10"/>
+  <dimension ref="A1:AF9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:AG1048576"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1460,12 +1466,12 @@
     <col min="27" max="27" width="17.81640625" customWidth="1"/>
     <col min="28" max="28" width="19.08984375" customWidth="1"/>
     <col min="29" max="29" width="17.81640625" customWidth="1"/>
-    <col min="30" max="32" width="17.81640625" style="21" customWidth="1"/>
-    <col min="33" max="33" width="30.90625" style="21" customWidth="1"/>
-    <col min="34" max="34" width="17.54296875" customWidth="1"/>
+    <col min="30" max="30" width="17.81640625" style="21" customWidth="1"/>
+    <col min="31" max="31" width="30.90625" style="21" customWidth="1"/>
+    <col min="32" max="32" width="17.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1554,22 +1560,16 @@
         <v>92</v>
       </c>
       <c r="AD1" s="21" t="s">
-        <v>123</v>
+        <v>169</v>
       </c>
       <c r="AE1" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="AF1" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="AG1" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="AH1" s="26" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AF1" s="26" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>105</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>107</v>
       </c>
       <c r="T2" s="21" t="s">
-        <v>108</v>
+        <v>168</v>
       </c>
       <c r="U2" s="21" t="s">
         <v>105</v>
@@ -1658,19 +1658,13 @@
         <v>106</v>
       </c>
       <c r="AD2" s="21" t="s">
-        <v>107</v>
+        <v>168</v>
       </c>
       <c r="AE2" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="AF2" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="AG2" s="21" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:32" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>60</v>
       </c>
@@ -1762,22 +1756,16 @@
         <v>89</v>
       </c>
       <c r="AE3" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="AF3" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="AG3" s="22" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="B4" s="23" t="str">
         <f t="shared" ref="B4" si="0">A4</f>
-        <v>2000084</v>
+        <v>1000092</v>
       </c>
       <c r="C4" s="23" t="s">
         <v>43</v>
@@ -1804,12 +1792,12 @@
         <v>13</v>
       </c>
       <c r="K4" s="23" t="str">
-        <f t="shared" ref="K4:L5" si="1">$A4</f>
-        <v>2000084</v>
+        <f t="shared" ref="K4:L4" si="1">$A4</f>
+        <v>1000092</v>
       </c>
       <c r="L4" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>2000084</v>
+        <v>1000092</v>
       </c>
       <c r="M4" s="23" t="s">
         <v>93</v>
@@ -1819,7 +1807,7 @@
       </c>
       <c r="O4" s="23" t="str">
         <f t="shared" ref="O4" si="2">A4</f>
-        <v>2000084</v>
+        <v>1000092</v>
       </c>
       <c r="P4" s="21" t="s">
         <v>19</v>
@@ -1834,135 +1822,56 @@
         <v>51</v>
       </c>
       <c r="U4" s="23" t="str">
-        <f t="shared" ref="U4:W5" si="3">$A4</f>
-        <v>2000084</v>
+        <f t="shared" ref="U4:W4" si="3">$A4</f>
+        <v>1000092</v>
       </c>
       <c r="V4" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>2000084</v>
+        <v>1000092</v>
       </c>
       <c r="W4" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>2000084</v>
+        <v>1000092</v>
       </c>
       <c r="X4" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="AE4" s="21" t="s">
+      <c r="AD4" s="21" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B5" s="23" t="str">
-        <f t="shared" ref="B5" si="4">A5</f>
-        <v>2000085</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="I5" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>2000085</v>
-      </c>
-      <c r="L5" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>2000085</v>
-      </c>
-      <c r="M5" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="N5" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="O5" s="23" t="str">
-        <f t="shared" ref="O5" si="5">A5</f>
-        <v>2000085</v>
-      </c>
-      <c r="P5" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q5" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="R5" s="21">
-        <v>11111</v>
-      </c>
-      <c r="T5" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="U5" s="23" t="str">
-        <f t="shared" si="3"/>
-        <v>2000085</v>
-      </c>
-      <c r="V5" s="23" t="str">
-        <f t="shared" si="3"/>
-        <v>2000085</v>
-      </c>
-      <c r="W5" s="23" t="str">
-        <f t="shared" si="3"/>
-        <v>2000085</v>
-      </c>
-      <c r="X5" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="AE5" s="21" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="AF4" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="K5" s="23"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="K6" s="23"/>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>143</v>
+      </c>
       <c r="K7" s="23"/>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="K8" s="23"/>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
-      <c r="A10" s="20" t="s">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A9" s="20" t="s">
         <v>147</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A10" r:id="rId1"/>
-    <hyperlink ref="N5" r:id="rId2"/>
-    <hyperlink ref="N4" r:id="rId3"/>
+    <hyperlink ref="A9" r:id="rId1"/>
+    <hyperlink ref="N4" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -3948,7 +3857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="O1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -4572,7 +4481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="W1" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add staging and prod environment
</commit_message>
<xml_diff>
--- a/trf-internal-user.xlsx
+++ b/trf-internal-user.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1341" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="192">
   <si>
     <t>Specimen ID Number</t>
   </si>
@@ -609,10 +609,16 @@
     <t>C:\Users\admin\Pictures\image(12086).png</t>
   </si>
   <si>
-    <t>2000088</t>
-  </si>
-  <si>
-    <t>2000089</t>
+    <t>Luong's Clinic - Patient Direct Bill</t>
+  </si>
+  <si>
+    <t>2000017</t>
+  </si>
+  <si>
+    <t>2000018</t>
+  </si>
+  <si>
+    <t>2000019</t>
   </si>
 </sst>
 </file>
@@ -1489,16 +1495,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI20"/>
+  <dimension ref="A1:AI13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.453125" customWidth="1"/>
+    <col min="2" max="2" width="37.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.08984375" style="21" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="15.08984375" style="21" customWidth="1"/>
     <col min="6" max="6" width="15.453125" bestFit="1" customWidth="1"/>
@@ -1841,14 +1847,14 @@
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B4" t="s">
         <v>187</v>
       </c>
       <c r="C4" s="23" t="str">
         <f>A4</f>
-        <v>2000088</v>
+        <v>2000017</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>43</v>
@@ -1876,11 +1882,11 @@
       </c>
       <c r="L4" s="23" t="str">
         <f>$A4</f>
-        <v>2000088</v>
+        <v>2000017</v>
       </c>
       <c r="M4" s="23" t="str">
         <f>$A4</f>
-        <v>2000088</v>
+        <v>2000017</v>
       </c>
       <c r="N4" s="23" t="s">
         <v>93</v>
@@ -1890,7 +1896,7 @@
       </c>
       <c r="P4" s="23" t="str">
         <f>A4</f>
-        <v>2000088</v>
+        <v>2000017</v>
       </c>
       <c r="Q4" s="21" t="s">
         <v>19</v>
@@ -1905,37 +1911,37 @@
         <v>51</v>
       </c>
       <c r="V4" s="23" t="str">
-        <f t="shared" ref="V4:X5" si="0">$A4</f>
-        <v>2000088</v>
+        <f t="shared" ref="V4:X6" si="0">$A4</f>
+        <v>2000017</v>
       </c>
       <c r="W4" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>2000088</v>
+        <v>2000017</v>
       </c>
       <c r="X4" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>2000088</v>
+        <v>2000017</v>
       </c>
       <c r="Y4" s="23" t="s">
         <v>110</v>
       </c>
       <c r="AF4" s="21" t="s">
-        <v>122</v>
+        <v>188</v>
       </c>
       <c r="AI4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B5" t="s">
         <v>187</v>
       </c>
       <c r="C5" s="23" t="str">
-        <f>A5</f>
-        <v>2000089</v>
+        <f t="shared" ref="C5:C6" si="1">A5</f>
+        <v>2000018</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>43</v>
@@ -1962,12 +1968,12 @@
         <v>13</v>
       </c>
       <c r="L5" s="23" t="str">
-        <f>$A5</f>
-        <v>2000089</v>
+        <f t="shared" ref="L5:M6" si="2">$A5</f>
+        <v>2000018</v>
       </c>
       <c r="M5" s="23" t="str">
-        <f>$A5</f>
-        <v>2000089</v>
+        <f t="shared" si="2"/>
+        <v>2000018</v>
       </c>
       <c r="N5" s="23" t="s">
         <v>93</v>
@@ -1976,8 +1982,8 @@
         <v>17</v>
       </c>
       <c r="P5" s="23" t="str">
-        <f>A5</f>
-        <v>2000089</v>
+        <f t="shared" ref="P5:P6" si="3">A5</f>
+        <v>2000018</v>
       </c>
       <c r="Q5" s="21" t="s">
         <v>19</v>
@@ -1993,47 +1999,112 @@
       </c>
       <c r="V5" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>2000089</v>
+        <v>2000018</v>
       </c>
       <c r="W5" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>2000089</v>
+        <v>2000018</v>
       </c>
       <c r="X5" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>2000089</v>
+        <v>2000018</v>
       </c>
       <c r="Y5" s="23" t="s">
         <v>110</v>
       </c>
       <c r="AF5" s="21" t="s">
-        <v>122</v>
+        <v>188</v>
       </c>
       <c r="AI5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" t="s">
+        <v>187</v>
+      </c>
+      <c r="C6" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>2000019</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="25"/>
-      <c r="P6" s="23"/>
-      <c r="R6" s="23"/>
-      <c r="V6" s="23"/>
-      <c r="W6" s="23"/>
-      <c r="X6" s="23"/>
-      <c r="Y6" s="23"/>
+      <c r="H6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>2000019</v>
+      </c>
+      <c r="M6" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>2000019</v>
+      </c>
+      <c r="N6" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="O6" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="P6" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>2000019</v>
+      </c>
+      <c r="Q6" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="R6" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="S6" s="21">
+        <v>11111</v>
+      </c>
+      <c r="U6" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="V6" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>2000019</v>
+      </c>
+      <c r="W6" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>2000019</v>
+      </c>
+      <c r="X6" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>2000019</v>
+      </c>
+      <c r="Y6" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF6" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="AI6" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
@@ -2124,126 +2195,30 @@
       <c r="Y10" s="23"/>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
+      <c r="A11" s="7" t="s">
+        <v>143</v>
+      </c>
       <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="23"/>
-      <c r="R11" s="23"/>
-      <c r="V11" s="23"/>
-      <c r="W11" s="23"/>
-      <c r="X11" s="23"/>
-      <c r="Y11" s="23"/>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="23"/>
-      <c r="R12" s="23"/>
-      <c r="V12" s="23"/>
-      <c r="W12" s="23"/>
-      <c r="X12" s="23"/>
-      <c r="Y12" s="23"/>
+      <c r="A12" s="7" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="23"/>
-      <c r="R13" s="23"/>
-      <c r="V13" s="23"/>
-      <c r="W13" s="23"/>
-      <c r="X13" s="23"/>
-      <c r="Y13" s="23"/>
-    </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="25"/>
-      <c r="P14" s="23"/>
-      <c r="R14" s="23"/>
-      <c r="V14" s="23"/>
-      <c r="W14" s="23"/>
-      <c r="X14" s="23"/>
-      <c r="Y14" s="23"/>
-    </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="L15" s="23"/>
-    </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="L16" s="23"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="L17" s="23"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A18" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="L18" s="23"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A19" s="7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A20" s="20" t="s">
+      <c r="A13" s="20" t="s">
         <v>147</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A20" r:id="rId1"/>
+    <hyperlink ref="A13" r:id="rId1"/>
     <hyperlink ref="O4" r:id="rId2"/>
     <hyperlink ref="O5" r:id="rId3"/>
+    <hyperlink ref="O6" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -2252,7 +2227,7 @@
   <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>